<commit_message>
html-css: BEM - block element modifier rule
</commit_message>
<xml_diff>
--- a/HTML_CSS.xlsx
+++ b/HTML_CSS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\202301_ReactJS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D048204-C53E-4881-BD53-09240B6FF8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9410CB06-EE85-46DC-A78D-D97308DD1B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Intro" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,10 @@
     <sheet name="2.CSS" sheetId="3" r:id="rId3"/>
     <sheet name="3.CSS" sheetId="5" r:id="rId4"/>
     <sheet name="4.Flexbox" sheetId="7" r:id="rId5"/>
-    <sheet name="Theshop" sheetId="8" r:id="rId6"/>
-    <sheet name="TheBand" sheetId="4" r:id="rId7"/>
-    <sheet name="QA1" sheetId="6" r:id="rId8"/>
+    <sheet name="5.BEM" sheetId="9" r:id="rId6"/>
+    <sheet name="Theshop" sheetId="8" r:id="rId7"/>
+    <sheet name="TheBand" sheetId="4" r:id="rId8"/>
+    <sheet name="QA1" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="446">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="494">
   <si>
     <t>HTML, CSS từ Zero tới Hero</t>
   </si>
@@ -1868,12 +1869,201 @@
   <si>
     <t>hoặc tự viết đơn giản --&gt;</t>
   </si>
+  <si>
+    <t>BEM là gì?</t>
+  </si>
+  <si>
+    <t>BEM</t>
+  </si>
+  <si>
+    <t>Là tiêu chuẩn đặt tên class khi viết CSS</t>
+  </si>
+  <si>
+    <t>Block Element Modifier</t>
+  </si>
+  <si>
+    <t>Cú pháp:</t>
+  </si>
+  <si>
+    <t>- .block</t>
+  </si>
+  <si>
+    <t>Tại sao cần BEM?</t>
+  </si>
+  <si>
+    <t>Modifier: class bổ sung ý nghĩa cho Block hoặc Element.</t>
+  </si>
+  <si>
+    <t>Member đặt tên class trùng nhau -&gt; CSS đè lên nhau</t>
+  </si>
+  <si>
+    <t>Mỗi người đặt tên một kiểu</t>
+  </si>
+  <si>
+    <t>- .block__element</t>
+  </si>
+  <si>
+    <t>- .block--modifier</t>
+  </si>
+  <si>
+    <t>- .block__element--modifier</t>
+  </si>
+  <si>
+    <t>Tính ứng dụng</t>
+  </si>
+  <si>
+    <t>Xây dựng layout Website</t>
+  </si>
+  <si>
+    <t>Ví dụ:</t>
+  </si>
+  <si>
+    <t>.card__heading</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.card </t>
+  </si>
+  <si>
+    <t>.card--success</t>
+  </si>
+  <si>
+    <t>.card__btn--large</t>
+  </si>
+  <si>
+    <t>Xây dựng thành phần trên Website</t>
+  </si>
+  <si>
+    <t>Ưu điểm:</t>
+  </si>
+  <si>
+    <t>- Dễ hiểu</t>
+  </si>
+  <si>
+    <t>- Tái sử dụng dễ dàng</t>
+  </si>
+  <si>
+    <t>- phù hợp teamwork</t>
+  </si>
+  <si>
+    <t>- Tính module, không lo trùng CSS</t>
+  </si>
+  <si>
+    <t>Nhược điểm:</t>
+  </si>
+  <si>
+    <t>- Tên class dài</t>
+  </si>
+  <si>
+    <t>Ưu/nhược điểm</t>
+  </si>
+  <si>
+    <t>Khi nào dùng BEM:</t>
+  </si>
+  <si>
+    <t>dự án nhiều members</t>
+  </si>
+  <si>
+    <t>dự án lớn, số lượng page nhiều hoặc số lượng thành phần trên giao diện nhiều</t>
+  </si>
+  <si>
+    <t>Trường hợp block lồng block</t>
+  </si>
+  <si>
+    <t>- Block con là thành phần dùng chung</t>
+  </si>
+  <si>
+    <t>&lt;div class="card"&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  &lt;div class="card__title"&gt;&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;/div&gt;</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ví dụ: btn dùng chung nhiều block -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dùng tên chung chứ ko thêm tiền tố block name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  &lt;div class="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>btn btn--primary pull-right</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF7030A0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&gt;&lt;/div&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>- Block con chứa nhiều element lồng nhau</t>
+  </si>
+  <si>
+    <t>Coi block con thành 1 block riêng.</t>
+  </si>
+  <si>
+    <t>.header</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ⇒ .navbar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ⇒ header-search </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ⇒ header-search__input</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ⇒ header-search__btn</t>
+  </si>
+  <si>
+    <t>// navbar coi như block riêng</t>
+  </si>
+  <si>
+    <t>// header-search coi như block riêng</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1952,6 +2142,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <i/>
       <sz val="11"/>
@@ -1988,7 +2186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2001,6 +2199,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4141,8 +4342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8F9F80-AB57-4CA4-A8C5-FDD5B3F3CCBA}">
   <dimension ref="A2:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I45" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4184,7 +4385,7 @@
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="12" t="s">
         <v>411</v>
       </c>
     </row>
@@ -4199,7 +4400,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="12" t="s">
         <v>410</v>
       </c>
     </row>
@@ -4214,7 +4415,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C22" s="11" t="s">
+      <c r="C22" s="12" t="s">
         <v>417</v>
       </c>
     </row>
@@ -4234,7 +4435,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="12" t="s">
         <v>418</v>
       </c>
     </row>
@@ -4262,7 +4463,7 @@
       <c r="A32" t="s">
         <v>432</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="12" t="s">
         <v>381</v>
       </c>
       <c r="E32" t="s">
@@ -4276,7 +4477,7 @@
       <c r="A33" t="s">
         <v>432</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" s="12" t="s">
         <v>382</v>
       </c>
       <c r="E33" t="s">
@@ -4284,7 +4485,7 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C34" s="11"/>
+      <c r="C34" s="12"/>
       <c r="I34" t="s">
         <v>433</v>
       </c>
@@ -4293,7 +4494,7 @@
       <c r="A35" t="s">
         <v>432</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" s="12" t="s">
         <v>383</v>
       </c>
       <c r="E35" t="s">
@@ -4307,7 +4508,7 @@
       <c r="A36" t="s">
         <v>432</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="12" t="s">
         <v>402</v>
       </c>
       <c r="I36" t="s">
@@ -4318,7 +4519,7 @@
       <c r="A37" t="s">
         <v>432</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="12" t="s">
         <v>385</v>
       </c>
       <c r="E37" t="s">
@@ -4326,7 +4527,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="11"/>
+      <c r="C38" s="12"/>
       <c r="I38" t="s">
         <v>431</v>
       </c>
@@ -4335,7 +4536,7 @@
       <c r="A39" t="s">
         <v>435</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="12" t="s">
         <v>427</v>
       </c>
       <c r="E39" t="s">
@@ -4349,7 +4550,7 @@
       <c r="A40" t="s">
         <v>432</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="12" t="s">
         <v>386</v>
       </c>
       <c r="E40" t="s">
@@ -4363,7 +4564,7 @@
       <c r="A41" t="s">
         <v>432</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="12" t="s">
         <v>428</v>
       </c>
       <c r="E41" t="s">
@@ -4371,7 +4572,7 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="C42" s="11"/>
+      <c r="C42" s="12"/>
       <c r="I42" t="s">
         <v>437</v>
       </c>
@@ -4380,7 +4581,7 @@
       <c r="A43" t="s">
         <v>435</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" s="12" t="s">
         <v>387</v>
       </c>
       <c r="E43" t="s">
@@ -4394,7 +4595,7 @@
       <c r="A44" t="s">
         <v>435</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" s="12" t="s">
         <v>384</v>
       </c>
       <c r="E44" t="s">
@@ -4408,7 +4609,7 @@
       <c r="A45" t="s">
         <v>435</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" s="12" t="s">
         <v>388</v>
       </c>
       <c r="E45" t="s">
@@ -4422,7 +4623,7 @@
       <c r="A46" t="s">
         <v>435</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" s="12" t="s">
         <v>389</v>
       </c>
       <c r="E46" t="s">
@@ -4436,7 +4637,7 @@
       <c r="A47" t="s">
         <v>435</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="12" t="s">
         <v>390</v>
       </c>
       <c r="E47" t="s">
@@ -4450,7 +4651,7 @@
       <c r="A48" t="s">
         <v>435</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" s="12" t="s">
         <v>391</v>
       </c>
       <c r="E48" t="s">
@@ -4467,6 +4668,253 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D5BE8F5-DE4C-4D1F-B7D3-0B7E1D820A82}">
+  <dimension ref="B2:J48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>450</v>
+      </c>
+      <c r="H16" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D17" s="6" t="s">
+        <v>451</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D18" s="6" t="s">
+        <v>456</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D19" s="6" t="s">
+        <v>457</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D20" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D25" s="7" t="s">
+        <v>467</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D26" s="6" t="s">
+        <v>468</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D27" s="6" t="s">
+        <v>469</v>
+      </c>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D28" s="6" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D29" s="6" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D35" s="6" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D36" s="6"/>
+      <c r="E36" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D37" s="6"/>
+      <c r="F37" s="5" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D38" s="6"/>
+      <c r="F38" s="5" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D39" s="6"/>
+      <c r="F39" s="5" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D40" s="6"/>
+      <c r="F40" s="13" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D42" s="6" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="E43" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F44" s="5" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F45" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="J45" s="14" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F46" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="J46" s="14" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F47" s="5" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="F48" s="5" t="s">
+        <v>491</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22CD8B08-E384-40E5-95F1-F89215990923}">
   <dimension ref="B2:I15"/>
   <sheetViews>
@@ -4531,7 +4979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8EF8412-9BF0-4D1F-B3A1-9D4DE092B57E}">
   <dimension ref="B2:I59"/>
   <sheetViews>
@@ -4856,7 +5304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D80607EF-8E5E-4B7C-AFBE-C633400FB2EE}">
   <dimension ref="B2:H41"/>
   <sheetViews>

</xml_diff>